<commit_message>
Further results for mgrid
</commit_message>
<xml_diff>
--- a/DIAs.xlsx
+++ b/DIAs.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
-    <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
+    <sheet name="12" sheetId="2" r:id="rId2"/>
+    <sheet name="40" sheetId="4" r:id="rId3"/>
+    <sheet name="Tabelle3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="56">
   <si>
     <t>nab Mem 1.3%</t>
   </si>
@@ -146,6 +147,45 @@
   <si>
     <t>30</t>
   </si>
+  <si>
+    <t>botsalgn Mem 0 %</t>
+  </si>
+  <si>
+    <t>applu331 Mem 45.2 %</t>
+  </si>
+  <si>
+    <t>smithwa Mem 0 %</t>
+  </si>
+  <si>
+    <t>kdtree Mem 0 %</t>
+  </si>
+  <si>
+    <t>botsspar Mem 0.8 %</t>
+  </si>
+  <si>
+    <t>nab Mem 0 %</t>
+  </si>
+  <si>
+    <t>fma3d Mem 0.6 %</t>
+  </si>
+  <si>
+    <t>imagick Mem  %</t>
+  </si>
+  <si>
+    <t>swim Mem 0.7 %</t>
+  </si>
+  <si>
+    <t>applu331 Mem 1.6 %</t>
+  </si>
+  <si>
+    <t>bt331 Mem 1.2 %</t>
+  </si>
+  <si>
+    <t>bwaves Mem  %</t>
+  </si>
+  <si>
+    <t>mgrid331 Mem %</t>
+  </si>
 </sst>
 </file>
 
@@ -212,7 +252,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1128,11 +1168,11 @@
         <c:hiLowLines/>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="212871424"/>
-        <c:axId val="217395584"/>
+        <c:axId val="183891072"/>
+        <c:axId val="183892992"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="212871424"/>
+        <c:axId val="183891072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1167,10 +1207,10 @@
             <a:pPr>
               <a:defRPr sz="1600"/>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="217395584"/>
+        <c:crossAx val="183892992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
@@ -1178,7 +1218,7 @@
         <c:minorUnit val="1"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="217395584"/>
+        <c:axId val="183892992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="26"/>
@@ -1198,10 +1238,10 @@
             <a:pPr>
               <a:defRPr sz="1600"/>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="212871424"/>
+        <c:crossAx val="183891072"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -1218,7 +1258,7 @@
           <a:pPr>
             <a:defRPr sz="1400"/>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1237,7 +1277,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1259,7 +1299,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle2!$A$2</c:f>
+              <c:f>'12'!$A$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1270,7 +1310,7 @@
           </c:tx>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle2!$B$2:$AE$2</c:f>
+              <c:f>'12'!$B$2:$AE$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -1374,7 +1414,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle2!$A$3</c:f>
+              <c:f>'12'!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1385,7 +1425,7 @@
           </c:tx>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle2!$B$3:$AE$3</c:f>
+              <c:f>'12'!$B$3:$AE$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -1489,7 +1529,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle2!$A$4</c:f>
+              <c:f>'12'!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1500,7 +1540,7 @@
           </c:tx>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle2!$B$4:$AE$4</c:f>
+              <c:f>'12'!$B$4:$AE$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -1604,7 +1644,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle2!$A$5</c:f>
+              <c:f>'12'!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1615,7 +1655,7 @@
           </c:tx>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle2!$B$5:$AE$5</c:f>
+              <c:f>'12'!$B$5:$AE$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -1719,7 +1759,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle2!$A$6</c:f>
+              <c:f>'12'!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1730,7 +1770,7 @@
           </c:tx>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle2!$B$6:$AE$6</c:f>
+              <c:f>'12'!$B$6:$AE$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -1834,7 +1874,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle2!$A$7</c:f>
+              <c:f>'12'!$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1845,7 +1885,7 @@
           </c:tx>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle2!$B$7:$AE$7</c:f>
+              <c:f>'12'!$B$7:$AE$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -1949,7 +1989,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle2!$A$8</c:f>
+              <c:f>'12'!$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1960,7 +2000,7 @@
           </c:tx>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle2!$B$8:$AE$8</c:f>
+              <c:f>'12'!$B$8:$AE$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -2064,7 +2104,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle2!$A$9</c:f>
+              <c:f>'12'!$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2075,7 +2115,7 @@
           </c:tx>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle2!$B$9:$AE$9</c:f>
+              <c:f>'12'!$B$9:$AE$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -2168,6 +2208,236 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>9.6141008174386915</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'12'!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>bt331 Mem 34 %</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>'12'!$B$10:$AE$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8868230547094427</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.7703432653772433</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.7612964277265202</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.5499379948488032</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.4629481159088309</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.3655411717603094</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.1832831325301205</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.8630069238377844</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.5333214062080689</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.7742825607064017</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.3725682845352729</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9.0886051829268286</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9.047230652503794</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9.5032875074716081</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.6221504942505547</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10.039360134708483</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10.187313114053824</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10.496698943661972</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10.699192462987886</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10.917143511100939</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>11.082016728624536</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>11.386249701599427</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>11.529369108049311</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>11.236042402826856</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>11.151975683890578</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>11.141555711282411</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>11.084592145015106</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>11.172874209416726</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>11.087168758716876</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'12'!$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>applu331 Mem 45.2 %</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>'12'!$B$11:$AE$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.800476284977178</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.6393786001047301</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.5266267589209361</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.2912685649418219</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0724589064072463</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.8412310069533868</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.6397833723653399</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.2488015340364331</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.6665539969579175</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.166156615661567</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.1485539788036636</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.9950655358519658</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.1539189402302474</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.401370533529124</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.8225556130367302</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.0388091440723013</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.2824538981194085</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.6175911854103351</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8.9104301708898053</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.1457661290322587</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.3647811725846406</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9.5986034701650436</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9.7976241900647949</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7.9682065694712803</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7.6795327577450481</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7.4992560753843609</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7.4831738700098978</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7.4757745550428476</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7.4451009354997542</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2176,10 +2446,10 @@
         </c:ser>
         <c:ser>
           <c:idx val="8"/>
-          <c:order val="8"/>
+          <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle2!$A$10</c:f>
+              <c:f>'12'!$A$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2190,7 +2460,7 @@
           </c:tx>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle2!$B$10:$AE$10</c:f>
+              <c:f>'12'!$B$12:$AE$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -2299,11 +2569,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="213051648"/>
-        <c:axId val="213356928"/>
+        <c:axId val="184934400"/>
+        <c:axId val="184936320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="213051648"/>
+        <c:axId val="184934400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2331,7 +2601,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213356928"/>
+        <c:crossAx val="184936320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2339,7 +2609,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="213356928"/>
+        <c:axId val="184936320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16"/>
@@ -2370,7 +2640,1106 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213051648"/>
+        <c:crossAx val="184934400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'40'!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>botsalgn Mem 0 %</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'40'!$B$14:$K$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'40'!$B$2:$K$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.9596774193548381</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19.944099378881987</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29.842007434944239</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>38.455089820359284</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40.542929292929294</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41.919060052219322</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43.158602150537632</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44.228650137741049</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44.412171507607191</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'40'!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>smithwa Mem 0 %</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'40'!$B$14:$K$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'40'!$B$3:$K$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.9193857965451055</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19.600505689001263</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28.817843866171003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>38.281481481481478</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>36.055813953488375</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38.76</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35.478260869565219</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>29.142857142857142</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>27.735241502683362</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'40'!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>kdtree Mem 0 %</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'40'!$B$14:$K$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'40'!$B$4:$K$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.798621745788668</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.991071428571429</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18.351351351351351</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22.558139534883722</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>26.73228346456693</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31.338461538461537</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>33.950000000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>35.736842105263158</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>39.022988505747129</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'40'!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>nab Mem 0 %</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'40'!$B$14:$K$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'40'!$B$5:$K$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.3884692849949651</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.762072434607646</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.468178493050477</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26.132680320569904</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28.409486931268152</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30.537981269510926</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32.535476718403551</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>33.235560588901471</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>34.812574139976277</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'40'!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>imagick Mem  %</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'40'!$B$14:$K$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'40'!$B$6:$K$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>31.934076137418757</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>34.531124497991968</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>38.003314917127071</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>38.730855855855857</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'40'!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>fma3d Mem 0.6 %</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'40'!$B$14:$K$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'40'!$B$7:$K$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.572950440018527</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.912871287128713</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14.14281516309139</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.513872135102533</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'40'!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>swim Mem 0.7 %</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'40'!$B$14:$K$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'40'!$B$8:$J$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.1771616541353387</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.9354059764563836</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.5495934959349587</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.5391872278664724</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.3094900849858355</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11.187234042553191</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'40'!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>botsspar Mem 0.8 %</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'40'!$B$14:$K$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'40'!$B$9:$K$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.6895514908544218</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19.172533465542884</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26.761937716262977</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30.862729449321627</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>33.481385281385279</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>33.744328097731241</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>33.656222802436901</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'40'!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>bt331 Mem 1.2 %</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'40'!$B$14:$K$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'40'!$B$10:$K$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.739570552147239</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>29.504995836802664</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>28.101110229976211</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'40'!$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>mgrid331 Mem %</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>'40'!$B$11:$K$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.2413757909777505</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.2701126307321</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>17.01054902900983</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17.313567593948267</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'40'!$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>applu331 Mem 1.6 %</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'40'!$B$14:$K$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'40'!$B$12:$K$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.447347158631835</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>17.283623517537219</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'40'!$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>bwaves Mem  %</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'40'!$B$14:$K$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'40'!$B$13:$K$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.3862857614663753</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.6614508220363424</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.034850774461654</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.532508412026484</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15.111506186886645</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.771744277821625</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>17.304397394136807</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18.165327406394255</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="184998528"/>
+        <c:axId val="185000704"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="184998528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1200"/>
+                  <a:t># Worker Threads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="185000704"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="185000704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="46"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1200"/>
+                  <a:t>Speed-up</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="184998528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2435,19 +3804,56 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
       <xdr:colOff>617220</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Diagramm 2"/>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>617220</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2757,12 +4163,12 @@
       <selection sqref="A1:AE14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2770,7 +4176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2778,7 +4184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -2873,7 +4279,7 @@
         <v>13.088120468488567</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2929,7 +4335,7 @@
         <v>12.107814045499506</v>
       </c>
     </row>
-    <row r="5" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -3024,7 +4430,7 @@
         <v>10.454397394136809</v>
       </c>
     </row>
-    <row r="6" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -3119,7 +4525,7 @@
         <v>11.606096131301289</v>
       </c>
     </row>
-    <row r="7" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -3160,7 +4566,7 @@
         <v>10.507840772014475</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -3255,7 +4661,7 @@
         <v>7.7371086556169431</v>
       </c>
     </row>
-    <row r="9" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -3284,7 +4690,7 @@
         <v>5.2323287671232874</v>
       </c>
     </row>
-    <row r="10" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -3379,7 +4785,7 @@
         <v>9.6141008174386915</v>
       </c>
     </row>
-    <row r="11" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -3387,7 +4793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -3419,7 +4825,7 @@
         <v>1.5308515540990322</v>
       </c>
     </row>
-    <row r="13" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -3436,18 +4842,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE11"/>
+  <dimension ref="A1:AE13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I7" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -3455,7 +4861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3550,7 +4956,7 @@
         <v>13.088120468488567</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -3645,7 +5051,7 @@
         <v>4.7835091832747167</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -3740,7 +5146,7 @@
         <v>10.454397394136809</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -3835,7 +5241,7 @@
         <v>11.606096131301289</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -3930,7 +5336,7 @@
         <v>12.031767955801104</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -4025,7 +5431,7 @@
         <v>7.7371086556169431</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -4120,7 +5526,7 @@
         <v>6.5114217524718718</v>
       </c>
     </row>
-    <row r="9" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -4215,190 +5621,380 @@
         <v>9.6141008174386915</v>
       </c>
     </row>
-    <row r="10" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10">
+        <v>1.8868230547094427</v>
+      </c>
+      <c r="D10">
+        <v>2.7703432653772433</v>
+      </c>
+      <c r="E10">
+        <v>3.7612964277265202</v>
+      </c>
+      <c r="F10">
+        <v>4.5499379948488032</v>
+      </c>
+      <c r="G10">
+        <v>5.4629481159088309</v>
+      </c>
+      <c r="H10">
+        <v>6.3655411717603094</v>
+      </c>
+      <c r="I10">
+        <v>7.1832831325301205</v>
+      </c>
+      <c r="J10">
+        <v>7.8630069238377844</v>
+      </c>
+      <c r="K10">
+        <v>8.5333214062080689</v>
+      </c>
+      <c r="L10">
+        <v>8.7742825607064017</v>
+      </c>
+      <c r="M10">
+        <v>9.3725682845352729</v>
+      </c>
+      <c r="N10">
+        <v>9.0886051829268286</v>
+      </c>
+      <c r="O10">
+        <v>9.047230652503794</v>
+      </c>
+      <c r="P10">
+        <v>9.5032875074716081</v>
+      </c>
+      <c r="Q10">
+        <v>9.6221504942505547</v>
+      </c>
+      <c r="R10">
+        <v>10.039360134708483</v>
+      </c>
+      <c r="S10">
+        <v>10.187313114053824</v>
+      </c>
+      <c r="T10">
+        <v>10.496698943661972</v>
+      </c>
+      <c r="U10">
+        <v>10.699192462987886</v>
+      </c>
+      <c r="V10">
+        <v>10.917143511100939</v>
+      </c>
+      <c r="W10">
+        <v>11.082016728624536</v>
+      </c>
+      <c r="X10">
+        <v>11.386249701599427</v>
+      </c>
+      <c r="Y10">
+        <v>11.529369108049311</v>
+      </c>
+      <c r="Z10">
+        <v>11.236042402826856</v>
+      </c>
+      <c r="AA10">
+        <v>11.151975683890578</v>
+      </c>
+      <c r="AB10">
+        <v>11.141555711282411</v>
+      </c>
+      <c r="AC10">
+        <v>11.084592145015106</v>
+      </c>
+      <c r="AD10">
+        <v>11.172874209416726</v>
+      </c>
+      <c r="AE10">
+        <v>11.087168758716876</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1.800476284977178</v>
+      </c>
+      <c r="D11">
+        <v>2.6393786001047301</v>
+      </c>
+      <c r="E11">
+        <v>3.5266267589209361</v>
+      </c>
+      <c r="F11">
+        <v>4.2912685649418219</v>
+      </c>
+      <c r="G11">
+        <v>5.0724589064072463</v>
+      </c>
+      <c r="H11">
+        <v>5.8412310069533868</v>
+      </c>
+      <c r="I11">
+        <v>6.6397833723653399</v>
+      </c>
+      <c r="J11">
+        <v>7.2488015340364331</v>
+      </c>
+      <c r="K11">
+        <v>7.6665539969579175</v>
+      </c>
+      <c r="L11">
+        <v>8.166156615661567</v>
+      </c>
+      <c r="M11">
+        <v>8.1485539788036636</v>
+      </c>
+      <c r="N11">
+        <v>6.9950655358519658</v>
+      </c>
+      <c r="O11">
+        <v>7.1539189402302474</v>
+      </c>
+      <c r="P11">
+        <v>7.401370533529124</v>
+      </c>
+      <c r="Q11">
+        <v>7.8225556130367302</v>
+      </c>
+      <c r="R11">
+        <v>8.0388091440723013</v>
+      </c>
+      <c r="S11">
+        <v>8.2824538981194085</v>
+      </c>
+      <c r="T11">
+        <v>8.6175911854103351</v>
+      </c>
+      <c r="U11">
+        <v>8.9104301708898053</v>
+      </c>
+      <c r="V11">
+        <v>9.1457661290322587</v>
+      </c>
+      <c r="W11">
+        <v>9.3647811725846406</v>
+      </c>
+      <c r="X11">
+        <v>9.5986034701650436</v>
+      </c>
+      <c r="Y11">
+        <v>9.7976241900647949</v>
+      </c>
+      <c r="Z11">
+        <v>7.9682065694712803</v>
+      </c>
+      <c r="AA11">
+        <v>7.6795327577450481</v>
+      </c>
+      <c r="AB11">
+        <v>7.4992560753843609</v>
+      </c>
+      <c r="AC11">
+        <v>7.4831738700098978</v>
+      </c>
+      <c r="AD11">
+        <v>7.4757745550428476</v>
+      </c>
+      <c r="AE11">
+        <v>7.4451009354997542</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
         <v>1.6661223277909738</v>
       </c>
-      <c r="D10">
+      <c r="D12">
         <v>1.9782311726082933</v>
       </c>
-      <c r="E10">
+      <c r="E12">
         <v>2.7803790412486067</v>
       </c>
-      <c r="F10">
+      <c r="F12">
         <v>3.2497466338497176</v>
       </c>
-      <c r="G10">
+      <c r="G12">
         <v>3.8736733108982655</v>
       </c>
-      <c r="H10">
+      <c r="H12">
         <v>4.4158961243360224</v>
       </c>
-      <c r="I10">
+      <c r="I12">
         <v>4.9631840796019899</v>
       </c>
-      <c r="J10">
+      <c r="J12">
         <v>5.3956730769230772</v>
       </c>
-      <c r="K10">
+      <c r="K12">
         <v>5.7880350696235174</v>
       </c>
-      <c r="L10">
+      <c r="L12">
         <v>6.0217303822937627</v>
       </c>
-      <c r="M10">
+      <c r="M12">
         <v>6.7063041529728116</v>
       </c>
-      <c r="N10">
+      <c r="N12">
         <v>6.6674587850883711</v>
       </c>
-      <c r="O10">
+      <c r="O12">
         <v>6.819383259911894</v>
       </c>
-      <c r="P10">
+      <c r="P12">
         <v>7.075177304964539</v>
       </c>
-      <c r="Q10">
+      <c r="Q12">
         <v>7.293582453290008</v>
       </c>
-      <c r="R10">
+      <c r="R12">
         <v>7.4782608695652177</v>
       </c>
-      <c r="S10">
+      <c r="S12">
         <v>7.7373319544984485</v>
       </c>
-      <c r="T10">
+      <c r="T12">
         <v>7.9244483671668133</v>
       </c>
-      <c r="U10">
+      <c r="U12">
         <v>8.0842787682333874</v>
       </c>
-      <c r="V10">
+      <c r="V12">
         <v>8.3706880477344772</v>
       </c>
-      <c r="W10">
+      <c r="W12">
         <v>8.4177761110069387</v>
       </c>
-      <c r="X10">
+      <c r="X12">
         <v>8.5671755725190835</v>
       </c>
-      <c r="Y10">
+      <c r="Y12">
         <v>8.7457627118644066</v>
       </c>
-      <c r="Z10">
+      <c r="Z12">
         <v>8.7542901716068648</v>
       </c>
-      <c r="AA10">
+      <c r="AA12">
         <v>8.5967062428188434</v>
       </c>
-      <c r="AB10">
+      <c r="AB12">
         <v>8.6463790446841298</v>
       </c>
-      <c r="AC10">
+      <c r="AC12">
         <v>8.5851979345955254</v>
       </c>
-      <c r="AD10">
+      <c r="AD12">
         <v>8.6032962821004215</v>
       </c>
-      <c r="AE10">
+      <c r="AE12">
         <v>8.7185861332297527</v>
       </c>
     </row>
-    <row r="11" spans="1:31" ht="15" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="K13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="L13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="M11" s="2" t="s">
+      <c r="M13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="N11" s="2" t="s">
+      <c r="N13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="O11" s="2" t="s">
+      <c r="O13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="P11" s="2" t="s">
+      <c r="P13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="Q11" s="2" t="s">
+      <c r="Q13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="R11" s="2" t="s">
+      <c r="R13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="S11" s="2" t="s">
+      <c r="S13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="T11" s="2" t="s">
+      <c r="T13" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="U11" s="2" t="s">
+      <c r="U13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="V11" s="2" t="s">
+      <c r="V13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="W11" s="2" t="s">
+      <c r="W13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="X11" s="2" t="s">
+      <c r="X13" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="Y11" s="2" t="s">
+      <c r="Y13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="Z11" s="2" t="s">
+      <c r="Z13" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AA11" s="2" t="s">
+      <c r="AA13" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AB11" s="2" t="s">
+      <c r="AB13" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AC11" s="2" t="s">
+      <c r="AC13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AD11" s="2" t="s">
+      <c r="AD13" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AE11" s="2" t="s">
+      <c r="AE13" s="2" t="s">
         <v>42</v>
       </c>
     </row>
@@ -4410,11 +6006,411 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AE14"/>
+  <sheetViews>
+    <sheetView topLeftCell="O16" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>9.9596774193548381</v>
+      </c>
+      <c r="D2">
+        <v>19.944099378881987</v>
+      </c>
+      <c r="E2">
+        <v>29.842007434944239</v>
+      </c>
+      <c r="F2">
+        <v>38.455089820359284</v>
+      </c>
+      <c r="G2">
+        <v>40.542929292929294</v>
+      </c>
+      <c r="H2">
+        <v>41.919060052219322</v>
+      </c>
+      <c r="I2">
+        <v>43.158602150537632</v>
+      </c>
+      <c r="J2">
+        <v>44.228650137741049</v>
+      </c>
+      <c r="K2">
+        <v>44.412171507607191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>9.9193857965451055</v>
+      </c>
+      <c r="D3">
+        <v>19.600505689001263</v>
+      </c>
+      <c r="E3">
+        <v>28.817843866171003</v>
+      </c>
+      <c r="F3">
+        <v>38.281481481481478</v>
+      </c>
+      <c r="G3">
+        <v>36.055813953488375</v>
+      </c>
+      <c r="H3">
+        <v>38.76</v>
+      </c>
+      <c r="I3">
+        <v>35.478260869565219</v>
+      </c>
+      <c r="J3">
+        <v>29.142857142857142</v>
+      </c>
+      <c r="K3">
+        <v>27.735241502683362</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>7.798621745788668</v>
+      </c>
+      <c r="D4">
+        <v>12.991071428571429</v>
+      </c>
+      <c r="E4">
+        <v>18.351351351351351</v>
+      </c>
+      <c r="F4">
+        <v>22.558139534883722</v>
+      </c>
+      <c r="G4">
+        <v>26.73228346456693</v>
+      </c>
+      <c r="H4">
+        <v>31.338461538461537</v>
+      </c>
+      <c r="I4">
+        <v>33.950000000000003</v>
+      </c>
+      <c r="J4">
+        <v>35.736842105263158</v>
+      </c>
+      <c r="K4">
+        <v>39.022988505747129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>7.3884692849949651</v>
+      </c>
+      <c r="D5">
+        <v>14.762072434607646</v>
+      </c>
+      <c r="E5">
+        <v>21.468178493050477</v>
+      </c>
+      <c r="F5">
+        <v>26.132680320569904</v>
+      </c>
+      <c r="G5">
+        <v>28.409486931268152</v>
+      </c>
+      <c r="H5">
+        <v>30.537981269510926</v>
+      </c>
+      <c r="I5">
+        <v>32.535476718403551</v>
+      </c>
+      <c r="J5">
+        <v>33.235560588901471</v>
+      </c>
+      <c r="K5">
+        <v>34.812574139976277</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>31.934076137418757</v>
+      </c>
+      <c r="G6">
+        <v>34.531124497991968</v>
+      </c>
+      <c r="J6">
+        <v>38.003314917127071</v>
+      </c>
+      <c r="K6">
+        <v>38.730855855855857</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>5.572950440018527</v>
+      </c>
+      <c r="F7">
+        <v>11.912871287128713</v>
+      </c>
+      <c r="J7">
+        <v>14.14281516309139</v>
+      </c>
+      <c r="K7">
+        <v>14.513872135102533</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>6.1771616541353387</v>
+      </c>
+      <c r="D8">
+        <v>7.9354059764563836</v>
+      </c>
+      <c r="F8">
+        <v>8.5495934959349587</v>
+      </c>
+      <c r="G8">
+        <v>9.5391872278664724</v>
+      </c>
+      <c r="H8">
+        <v>9.3094900849858355</v>
+      </c>
+      <c r="J8">
+        <v>11.187234042553191</v>
+      </c>
+      <c r="K8">
+        <v>11.470331588132636</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>9.6895514908544218</v>
+      </c>
+      <c r="D9">
+        <v>19.172533465542884</v>
+      </c>
+      <c r="E9">
+        <v>26.761937716262977</v>
+      </c>
+      <c r="F9">
+        <v>30.862729449321627</v>
+      </c>
+      <c r="G9">
+        <v>33.481385281385279</v>
+      </c>
+      <c r="J9">
+        <v>33.744328097731241</v>
+      </c>
+      <c r="K9">
+        <v>33.656222802436901</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>21.739570552147239</v>
+      </c>
+      <c r="J10">
+        <v>29.504995836802664</v>
+      </c>
+      <c r="K10">
+        <v>28.101110229976211</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>7.2413757909777505</v>
+      </c>
+      <c r="F11">
+        <v>14.2701126307321</v>
+      </c>
+      <c r="J11">
+        <v>17.01054902900983</v>
+      </c>
+      <c r="K11">
+        <v>17.313567593948267</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>18.447347158631835</v>
+      </c>
+      <c r="J12">
+        <v>17.283623517537219</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>4.3862857614663753</v>
+      </c>
+      <c r="D13">
+        <v>7.6614508220363424</v>
+      </c>
+      <c r="E13">
+        <v>10.034850774461654</v>
+      </c>
+      <c r="F13">
+        <v>11.532508412026484</v>
+      </c>
+      <c r="H13">
+        <v>15.111506186886645</v>
+      </c>
+      <c r="I13">
+        <v>16.771744277821625</v>
+      </c>
+      <c r="J13">
+        <v>17.304397394136807</v>
+      </c>
+      <c r="K13">
+        <v>18.165327406394255</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="2">
+        <v>10</v>
+      </c>
+      <c r="D14" s="2">
+        <v>20</v>
+      </c>
+      <c r="E14" s="2">
+        <v>30</v>
+      </c>
+      <c r="F14" s="2">
+        <v>40</v>
+      </c>
+      <c r="G14" s="2">
+        <v>50</v>
+      </c>
+      <c r="H14" s="2">
+        <v>60</v>
+      </c>
+      <c r="I14" s="2">
+        <v>70</v>
+      </c>
+      <c r="J14" s="2">
+        <v>80</v>
+      </c>
+      <c r="K14" s="2">
+        <v>90</v>
+      </c>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2"/>
+      <c r="AA14" s="2"/>
+      <c r="AB14" s="2"/>
+      <c r="AC14" s="2"/>
+      <c r="AD14" s="2"/>
+      <c r="AE14" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
md except of two
</commit_message>
<xml_diff>
--- a/DIAs.xlsx
+++ b/DIAs.xlsx
@@ -1171,11 +1171,11 @@
         <c:hiLowLines/>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="175179648"/>
-        <c:axId val="177214976"/>
+        <c:axId val="215196416"/>
+        <c:axId val="215198336"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="175179648"/>
+        <c:axId val="215196416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1213,7 +1213,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="177214976"/>
+        <c:crossAx val="215198336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
@@ -1221,7 +1221,7 @@
         <c:minorUnit val="1"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="177214976"/>
+        <c:axId val="215198336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="26"/>
@@ -1244,7 +1244,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="175179648"/>
+        <c:crossAx val="215196416"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -2687,11 +2687,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="220241280"/>
-        <c:axId val="220386048"/>
+        <c:axId val="214876544"/>
+        <c:axId val="214878464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="220241280"/>
+        <c:axId val="214876544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2713,13 +2713,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="220386048"/>
+        <c:crossAx val="214878464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2727,7 +2726,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="220386048"/>
+        <c:axId val="214878464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16"/>
@@ -2751,21 +2750,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="220241280"/>
+        <c:crossAx val="214876544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2920,6 +2917,9 @@
                 <c:pt idx="2">
                   <c:v>2.254697633168893</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.5879765395894427</c:v>
+                </c:pt>
                 <c:pt idx="6">
                   <c:v>5.2136631632914634</c:v>
                 </c:pt>
@@ -3981,11 +3981,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="145408768"/>
-        <c:axId val="145410688"/>
+        <c:axId val="215061248"/>
+        <c:axId val="215063168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="145408768"/>
+        <c:axId val="215061248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4014,7 +4014,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145410688"/>
+        <c:crossAx val="215063168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4022,7 +4022,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="145410688"/>
+        <c:axId val="215063168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="46"/>
@@ -4054,7 +4054,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145408768"/>
+        <c:crossAx val="215061248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6418,8 +6418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J18" workbookViewId="0">
-      <selection activeCell="AB17" sqref="AB17"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6436,6 +6436,9 @@
       </c>
       <c r="D1">
         <v>2.254697633168893</v>
+      </c>
+      <c r="G1">
+        <v>4.5879765395894427</v>
       </c>
       <c r="H1">
         <v>5.2136631632914634</v>

</xml_diff>